<commit_message>
testing for errors found.
</commit_message>
<xml_diff>
--- a/userDownload/planner.xlsx
+++ b/userDownload/planner.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Meal Plan BMR= BMI=</t>
   </si>
@@ -44,36 +44,7 @@
     <t> Saturday</t>
   </si>
   <si>
-    <t>New Meal</t>
-  </si>
-  <si>
-    <t>GREEK YOGURT (1.0 CUP)
-APPLE (1.0 MEDIUM)</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>CRAB (6.0 0Z)
-HALIBUT (2.0 0Z)</t>
-  </si>
-  <si>
-    <t>k k</t>
-  </si>
-  <si>
-    <t>ARBYS, roast beef sandwich, classic (3.0 sandwich)</t>
-  </si>
-  <si>
-    <t>new lunch</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
     <t>Calories</t>
-  </si>
-  <si>
-    <t>1,083.0</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -241,7 +212,7 @@
       <name val="arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,24 +240,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000FFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -321,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -385,19 +338,7 @@
     <xf xfId="0" fontId="14" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="14" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="14" numFmtId="0" fillId="6" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="14" numFmtId="0" fillId="7" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="14" numFmtId="0" fillId="8" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="10"/>
-    </xf>
-    <xf xfId="0" fontId="15" numFmtId="0" fillId="8" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="15" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -735,10 +676,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J995"/>
+  <dimension ref="A1:J990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="14.43" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -799,154 +740,81 @@
     </row>
     <row r="3" spans="1:10" customHeight="1" ht="14.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" customHeight="1" ht="14.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="1:10" customHeight="1" ht="22.5">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="5"/>
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" customHeight="1" ht="14.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="1:10" customHeight="1" ht="12.75">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" customHeight="1" ht="36.75">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="5"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="15"/>
     </row>
-    <row r="6" spans="1:10" customHeight="1" ht="14.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" customHeight="1" ht="14.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" customHeight="1" ht="14.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" customHeight="1" ht="22.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="25">
-        <v>0</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="25">
-        <v>223</v>
-      </c>
-      <c r="F9" s="25">
-        <v>0</v>
-      </c>
-      <c r="G9" s="25">
-        <v>204.7</v>
-      </c>
-      <c r="H9" s="25">
-        <v>0</v>
-      </c>
-      <c r="I9" s="25">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" customHeight="1" ht="12.75">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" customHeight="1" ht="36.75">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="15"/>
-    </row>
+    <row r="7" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="8" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="9" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="10" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="11" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="12" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="13" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="14" spans="1:10" customHeight="1" ht="15.75"/>
@@ -1926,16 +1794,11 @@
     <row r="988" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="989" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="990" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="991" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="992" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="993" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="994" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="995" spans="1:10" customHeight="1" ht="15.75"/>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <printOptions gridLines="true" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
add gdrive link to download sheets document.
</commit_message>
<xml_diff>
--- a/userDownload/planner.xlsx
+++ b/userDownload/planner.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Meal Plan BMR= BMI=</t>
   </si>
@@ -44,7 +44,36 @@
     <t> Saturday</t>
   </si>
   <si>
+    <t>New Meal</t>
+  </si>
+  <si>
+    <t>GREEK YOGURT (1.0 CUP)
+APPLE (1.0 MEDIUM)</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>CRAB (6.0 0Z)
+HALIBUT (2.0 0Z)</t>
+  </si>
+  <si>
+    <t>k k</t>
+  </si>
+  <si>
+    <t>ARBYS, roast beef sandwich, classic (3.0 sandwich)</t>
+  </si>
+  <si>
+    <t>new lunch</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
     <t>Calories</t>
+  </si>
+  <si>
+    <t>1,083.0</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -212,7 +241,7 @@
       <name val="arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +269,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -274,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -338,7 +385,19 @@
     <xf xfId="0" fontId="14" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="15" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="6" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="7" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="8" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="10"/>
+    </xf>
+    <xf xfId="0" fontId="15" numFmtId="0" fillId="8" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -676,10 +735,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J990"/>
+  <dimension ref="A1:J995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="14.43" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -740,81 +799,154 @@
     </row>
     <row r="3" spans="1:10" customHeight="1" ht="14.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" customHeight="1" ht="22.5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:10" customHeight="1" ht="14.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" customHeight="1" ht="14.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" customHeight="1" ht="14.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" customHeight="1" ht="14.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" customHeight="1" ht="14.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" customHeight="1" ht="22.5">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="25">
         <v>0</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="25">
+        <v>223</v>
+      </c>
+      <c r="F9" s="25">
         <v>0</v>
       </c>
-      <c r="E4" s="21">
+      <c r="G9" s="25">
+        <v>204.7</v>
+      </c>
+      <c r="H9" s="25">
         <v>0</v>
       </c>
-      <c r="F4" s="21">
+      <c r="I9" s="25">
         <v>0</v>
       </c>
-      <c r="G4" s="21">
-        <v>0</v>
-      </c>
-      <c r="H4" s="21">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11"/>
+      <c r="J9" s="11"/>
     </row>
-    <row r="5" spans="1:10" customHeight="1" ht="12.75">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="12"/>
+    <row r="10" spans="1:10" customHeight="1" ht="12.75">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="12"/>
     </row>
-    <row r="6" spans="1:10" customHeight="1" ht="36.75">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="15"/>
+    <row r="11" spans="1:10" customHeight="1" ht="36.75">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="15"/>
     </row>
-    <row r="7" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="8" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="9" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="10" spans="1:10" customHeight="1" ht="15.75"/>
-    <row r="11" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="12" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="13" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="14" spans="1:10" customHeight="1" ht="15.75"/>
@@ -1794,11 +1926,16 @@
     <row r="988" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="989" spans="1:10" customHeight="1" ht="15.75"/>
     <row r="990" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="991" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="992" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="993" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="994" spans="1:10" customHeight="1" ht="15.75"/>
+    <row r="995" spans="1:10" customHeight="1" ht="15.75"/>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="G11:I11"/>
   </mergeCells>
   <printOptions gridLines="true" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
update planner to local settings.
</commit_message>
<xml_diff>
--- a/userDownload/planner.xlsx
+++ b/userDownload/planner.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Meal Plan BMR= BMI=</t>
   </si>
@@ -45,23 +45,28 @@
   </si>
   <si>
     <t>New Meal</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>HALIBUT (2.0 0Z)
+CRAB (6.0 0Z)</t>
+  </si>
+  <si>
+    <t>k k</t>
+  </si>
+  <si>
+    <t>EZEKIEL BREAD (1.0 SLICE)
+ARBYS, roast beef sandwich, classic (3.0 sandwich)</t>
   </si>
   <si>
     <t>GREEK YOGURT (1.0 CUP)
 APPLE (1.0 MEDIUM)</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>CRAB (6.0 0Z)
-HALIBUT (2.0 0Z)</t>
-  </si>
-  <si>
-    <t>k k</t>
-  </si>
-  <si>
-    <t>ARBYS, roast beef sandwich, classic (3.0 sandwich)</t>
+    <t>APPLE (1.0 MEDIUM)
+GREEK YOGURT (1.0 CUP)</t>
   </si>
   <si>
     <t>new lunch</t>
@@ -73,7 +78,7 @@
     <t>Calories</t>
   </si>
   <si>
-    <t>1,083.0</t>
+    <t>1,163.0</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -804,9 +809,7 @@
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
-        <v>10</v>
-      </c>
+      <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
@@ -830,14 +833,14 @@
     <row r="5" spans="1:10" customHeight="1" ht="14.25">
       <c r="A5" s="5"/>
       <c r="B5" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
@@ -846,23 +849,27 @@
     <row r="6" spans="1:10" customHeight="1" ht="14.25">
       <c r="A6" s="5"/>
       <c r="B6" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="I6" s="24"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" customHeight="1" ht="14.25">
       <c r="A7" s="5"/>
       <c r="B7" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -876,7 +883,7 @@
     <row r="8" spans="1:10" customHeight="1" ht="14.25">
       <c r="A8" s="5"/>
       <c r="B8" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -890,25 +897,25 @@
     <row r="9" spans="1:10" customHeight="1" ht="22.5">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="25">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
         <v>223</v>
-      </c>
-      <c r="F9" s="25">
-        <v>0</v>
       </c>
       <c r="G9" s="25">
         <v>204.7</v>
       </c>
       <c r="H9" s="25">
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="I9" s="25">
         <v>0</v>
@@ -918,14 +925,14 @@
     <row r="10" spans="1:10" customHeight="1" ht="12.75">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -934,14 +941,14 @@
     <row r="11" spans="1:10" customHeight="1" ht="36.75">
       <c r="A11" s="15"/>
       <c r="B11" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>

</xml_diff>